<commit_message>
Updated the UI a little more and multple json file injection
</commit_message>
<xml_diff>
--- a/tools/data/terms.xlsx
+++ b/tools/data/terms.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\workbench\HTML\tech-explainer\tools\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF520DA1-53BF-4401-B73E-AA2C3F987591}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A75173A3-90F6-4D95-8747-6E5202B80DBB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="raw" sheetId="1" r:id="rId1"/>
@@ -11203,8 +11203,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:A3500"/>
   <sheetViews>
-    <sheetView topLeftCell="A3434" workbookViewId="0">
-      <selection sqref="A1:A3500"/>
+    <sheetView topLeftCell="A844" workbookViewId="0">
+      <selection activeCell="M859" sqref="M859"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -28817,8 +28817,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:J51"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J1" sqref="A1:J1"/>
+    <sheetView topLeftCell="A12" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E48" sqref="E48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -30446,8 +30446,8 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:J51"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J1" sqref="A1:J1"/>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="G41" sqref="G41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -33731,7 +33731,7 @@
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:J51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>

</xml_diff>